<commit_message>
Python tool to generate json for story complete
</commit_message>
<xml_diff>
--- a/project-CB-Story.xlsx
+++ b/project-CB-Story.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bm199305/Git/Project-CB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{477FA47C-DB49-C645-A63C-DEAB49FF84AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BCE57F-23FE-4049-92F0-48588774228E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5740" yWindow="8280" windowWidth="28040" windowHeight="17440" xr2:uid="{92FAE594-B098-0746-80A6-1E68B077A383}"/>
+    <workbookView xWindow="-31780" yWindow="2460" windowWidth="28040" windowHeight="17440" xr2:uid="{92FAE594-B098-0746-80A6-1E68B077A383}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>gameTime</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>This is a test story point 3</t>
+  </si>
+  <si>
+    <t>This is a different story point on 2</t>
   </si>
 </sst>
 </file>
@@ -432,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBFCD878-2F82-A443-BEE5-1D2E43DBC441}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -501,6 +504,20 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>